<commit_message>
position, work station switch
</commit_message>
<xml_diff>
--- a/upload/data.xlsx
+++ b/upload/data.xlsx
@@ -12398,8 +12398,8 @@
   </sheetPr>
   <dimension ref="A1:S742"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="53.25" customHeight="1"/>
@@ -12407,7 +12407,7 @@
     <col min="1" max="1" width="5.5546875" style="98" customWidth="1"/>
     <col min="2" max="2" width="6.44140625" style="98" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="98" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="99" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="99" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" style="98" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" style="98" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="98" customWidth="1"/>

</xml_diff>